<commit_message>
split to chunks, add multiprocessing, concurrent futures
</commit_message>
<xml_diff>
--- a/report/report.xlsx
+++ b/report/report.xlsx
@@ -751,7 +751,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E11"/>
+  <dimension ref="A1:E24"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -759,7 +759,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="15.22" customWidth="1" min="1" max="1"/>
+    <col width="16.22" customWidth="1" min="1" max="1"/>
     <col width="16.22" customWidth="1" min="2" max="2"/>
     <col width="1.22" customWidth="1" min="3" max="3"/>
     <col width="16.22" customWidth="1" min="4" max="4"/>
@@ -792,11 +792,11 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Тольятти</t>
+          <t>Воронеж</t>
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>42962</v>
+        <v>73587</v>
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
@@ -804,17 +804,17 @@
         </is>
       </c>
       <c r="E2" s="3" t="n">
-        <v>0.3246</v>
+        <v>0.2461</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Волгоград</t>
+          <t>Ростов-на-Дону</t>
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>43120</v>
+        <v>76579</v>
       </c>
       <c r="D3" s="2" t="inlineStr">
         <is>
@@ -822,151 +822,329 @@
         </is>
       </c>
       <c r="E3" s="3" t="n">
-        <v>0.1197</v>
+        <v>0.1086</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>Ижевск</t>
+          <t>Казань</t>
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>43229</v>
+        <v>59991</v>
       </c>
       <c r="D4" s="2" t="inlineStr">
         <is>
-          <t>Новосибирск</t>
+          <t>Нижний Новгород</t>
         </is>
       </c>
       <c r="E4" s="3" t="n">
-        <v>0.0271</v>
+        <v>0.022</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>Воронеж</t>
+          <t>Нижний Новгород</t>
         </is>
       </c>
       <c r="B5" s="2" t="n">
-        <v>44505</v>
+        <v>76491</v>
       </c>
       <c r="D5" s="2" t="inlineStr">
         <is>
-          <t>Казань</t>
+          <t>Ростов-на-Дону</t>
         </is>
       </c>
       <c r="E5" s="3" t="n">
-        <v>0.0237</v>
+        <v>0.02</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="inlineStr">
         <is>
-          <t>Барнаул</t>
+          <t>Новосибирск</t>
         </is>
       </c>
       <c r="B6" s="2" t="n">
-        <v>44550</v>
+        <v>46820</v>
       </c>
       <c r="D6" s="2" t="inlineStr">
         <is>
-          <t>Нижний Новгород</t>
+          <t>Воронеж</t>
         </is>
       </c>
       <c r="E6" s="3" t="n">
-        <v>0.0232</v>
+        <v>0.0167</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="inlineStr">
         <is>
-          <t>Саратов</t>
+          <t>Екатеринбург</t>
         </is>
       </c>
       <c r="B7" s="2" t="n">
-        <v>44829</v>
+        <v>81550</v>
       </c>
       <c r="D7" s="2" t="inlineStr">
         <is>
-          <t>Ростов-на-Дону</t>
+          <t>Екатеринбург</t>
         </is>
       </c>
       <c r="E7" s="3" t="n">
-        <v>0.0209</v>
+        <v>0.0305</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="inlineStr">
         <is>
-          <t>Рязань</t>
+          <t>Санкт-Петербург</t>
         </is>
       </c>
       <c r="B8" s="2" t="n">
-        <v>45118</v>
+        <v>52774</v>
       </c>
       <c r="D8" s="2" t="inlineStr">
         <is>
-          <t>Екатеринбург</t>
+          <t>Казань</t>
         </is>
       </c>
       <c r="E8" s="3" t="n">
-        <v>0.0207</v>
+        <v>0.0269</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="inlineStr">
         <is>
-          <t>Ростов-на-Дону</t>
+          <t>Москва</t>
         </is>
       </c>
       <c r="B9" s="2" t="n">
-        <v>45202</v>
+        <v>51234</v>
       </c>
       <c r="D9" s="2" t="inlineStr">
         <is>
-          <t>Краснодар</t>
+          <t>Новосибирск</t>
         </is>
       </c>
       <c r="E9" s="3" t="n">
-        <v>0.0185</v>
+        <v>0.0308</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="inlineStr">
         <is>
-          <t>Тула</t>
+          <t>Россия</t>
         </is>
       </c>
       <c r="B10" s="2" t="n">
-        <v>45795</v>
+        <v>48221</v>
       </c>
       <c r="D10" s="2" t="inlineStr">
         <is>
-          <t>Самара</t>
+          <t>Россия</t>
         </is>
       </c>
       <c r="E10" s="3" t="n">
-        <v>0.0143</v>
+        <v>0.0224</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="inlineStr">
         <is>
+          <t>Самара</t>
+        </is>
+      </c>
+      <c r="B11" s="2" t="n">
+        <v>78886</v>
+      </c>
+      <c r="D11" s="2" t="inlineStr">
+        <is>
+          <t>Самара</t>
+        </is>
+      </c>
+      <c r="E11" s="3" t="n">
+        <v>0.0162</v>
+      </c>
+    </row>
+    <row r="12">
+      <c r="A12" s="2" t="inlineStr">
+        <is>
           <t>Ярославль</t>
         </is>
       </c>
-      <c r="B11" s="2" t="n">
-        <v>46233</v>
-      </c>
-      <c r="D11" s="2" t="inlineStr">
-        <is>
-          <t>Воронеж</t>
-        </is>
-      </c>
-      <c r="E11" s="3" t="n">
-        <v>0.0141</v>
+      <c r="B12" s="2" t="n">
+        <v>46273</v>
+      </c>
+      <c r="D12" s="2" t="inlineStr">
+        <is>
+          <t>Краснодар</t>
+        </is>
+      </c>
+      <c r="E12" s="2" t="n">
+        <v>0.0243</v>
+      </c>
+    </row>
+    <row r="13">
+      <c r="A13" s="2" t="inlineStr">
+        <is>
+          <t>Краснодар</t>
+        </is>
+      </c>
+      <c r="B13" s="2" t="n">
+        <v>82585</v>
+      </c>
+      <c r="D13" s="2" t="inlineStr">
+        <is>
+          <t>Ярославль</t>
+        </is>
+      </c>
+      <c r="E13" s="2" t="n">
+        <v>0.0127</v>
+      </c>
+    </row>
+    <row r="14">
+      <c r="A14" s="2" t="inlineStr">
+        <is>
+          <t>Пермь</t>
+        </is>
+      </c>
+      <c r="B14" s="2" t="n">
+        <v>81440</v>
+      </c>
+      <c r="D14" s="2" t="inlineStr">
+        <is>
+          <t>Красноярск</t>
+        </is>
+      </c>
+      <c r="E14" s="2" t="n">
+        <v>0.0145</v>
+      </c>
+    </row>
+    <row r="15">
+      <c r="A15" s="2" t="inlineStr">
+        <is>
+          <t>Красноярск</t>
+        </is>
+      </c>
+      <c r="B15" s="2" t="n">
+        <v>69883</v>
+      </c>
+      <c r="D15" s="2" t="inlineStr">
+        <is>
+          <t>Пермь</t>
+        </is>
+      </c>
+      <c r="E15" s="2" t="n">
+        <v>0.0165</v>
+      </c>
+    </row>
+    <row r="16">
+      <c r="A16" s="2" t="inlineStr">
+        <is>
+          <t>Волгоград</t>
+        </is>
+      </c>
+      <c r="B16" s="2" t="n">
+        <v>46518</v>
+      </c>
+      <c r="D16" s="2" t="inlineStr">
+        <is>
+          <t>Уфа</t>
+        </is>
+      </c>
+      <c r="E16" s="2" t="n">
+        <v>0.0152</v>
+      </c>
+    </row>
+    <row r="17">
+      <c r="A17" s="2" t="inlineStr">
+        <is>
+          <t>Уфа</t>
+        </is>
+      </c>
+      <c r="B17" s="2" t="n">
+        <v>79632</v>
+      </c>
+      <c r="D17" s="2" t="inlineStr">
+        <is>
+          <t>Челябинск</t>
+        </is>
+      </c>
+      <c r="E17" s="2" t="n">
+        <v>0.0167</v>
+      </c>
+    </row>
+    <row r="18">
+      <c r="A18" s="2" t="inlineStr">
+        <is>
+          <t>Саратов</t>
+        </is>
+      </c>
+      <c r="B18" s="2" t="n">
+        <v>50935</v>
+      </c>
+    </row>
+    <row r="19">
+      <c r="A19" s="2" t="inlineStr">
+        <is>
+          <t>Тула</t>
+        </is>
+      </c>
+      <c r="B19" s="2" t="n">
+        <v>44614</v>
+      </c>
+    </row>
+    <row r="20">
+      <c r="A20" s="2" t="inlineStr">
+        <is>
+          <t>Ижевск</t>
+        </is>
+      </c>
+      <c r="B20" s="2" t="n">
+        <v>44443</v>
+      </c>
+    </row>
+    <row r="21">
+      <c r="A21" s="2" t="inlineStr">
+        <is>
+          <t>Челябинск</t>
+        </is>
+      </c>
+      <c r="B21" s="2" t="n">
+        <v>70440</v>
+      </c>
+    </row>
+    <row r="22">
+      <c r="A22" s="2" t="inlineStr">
+        <is>
+          <t>Омск</t>
+        </is>
+      </c>
+      <c r="B22" s="2" t="n">
+        <v>49788</v>
+      </c>
+    </row>
+    <row r="23">
+      <c r="A23" s="2" t="inlineStr">
+        <is>
+          <t>Рязань</t>
+        </is>
+      </c>
+      <c r="B23" s="2" t="n">
+        <v>37293</v>
+      </c>
+    </row>
+    <row r="24">
+      <c r="A24" s="2" t="inlineStr">
+        <is>
+          <t>Тюмень</t>
+        </is>
+      </c>
+      <c r="B24" s="2" t="n">
+        <v>78655</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
add new statistics for proj
</commit_message>
<xml_diff>
--- a/report/report.xlsx
+++ b/report/report.xlsx
@@ -1,14 +1,14 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main">
   <workbookPr/>
   <workbookProtection/>
   <bookViews>
     <workbookView visibility="visible" minimized="0" showHorizontalScroll="1" showVerticalScroll="1" showSheetTabs="1" tabRatio="600" firstSheet="0" activeTab="0" autoFilterDateGrouping="1"/>
   </bookViews>
   <sheets>
-    <sheet name="Статистика по годам" sheetId="1" state="visible" r:id="rId1"/>
-    <sheet name="Статистика по городам" sheetId="2" state="visible" r:id="rId2"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Статистика по годам" sheetId="1" state="visible" r:id="rId1"/>
+    <sheet xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" name="Статистика по городам" sheetId="2" state="visible" r:id="rId2"/>
   </sheets>
   <definedNames/>
   <calcPr calcId="124519" fullCalcOnLoad="1"/>
@@ -426,7 +426,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E17"/>
+  <dimension ref="A1:E9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -436,9 +436,9 @@
   <cols>
     <col width="5.22" customWidth="1" min="1" max="1"/>
     <col width="17.22" customWidth="1" min="2" max="2"/>
-    <col width="31.22" customWidth="1" min="3" max="3"/>
+    <col width="35.22" customWidth="1" min="3" max="3"/>
     <col width="20.22" customWidth="1" min="4" max="4"/>
-    <col width="34.22" customWidth="1" min="5" max="5"/>
+    <col width="38.22" customWidth="1" min="5" max="5"/>
   </cols>
   <sheetData>
     <row r="1">
@@ -454,7 +454,7 @@
       </c>
       <c r="C1" s="1" t="inlineStr">
         <is>
-          <t>Средняя зарплата - Программист</t>
+          <t>Средняя зарплата - web разработчик</t>
         </is>
       </c>
       <c r="D1" s="1" t="inlineStr">
@@ -464,280 +464,144 @@
       </c>
       <c r="E1" s="1" t="inlineStr">
         <is>
-          <t>Количество вакансий - Программист</t>
+          <t>Количество вакансий - web разработчик</t>
         </is>
       </c>
     </row>
     <row r="2">
       <c r="A2" s="2" t="n">
-        <v>2007</v>
+        <v>2015</v>
       </c>
       <c r="B2" s="2" t="n">
-        <v>38916</v>
+        <v>57212</v>
       </c>
       <c r="C2" s="2" t="n">
-        <v>43770</v>
+        <v>57150</v>
       </c>
       <c r="D2" s="2" t="n">
-        <v>2196</v>
+        <v>9397</v>
       </c>
       <c r="E2" s="2" t="n">
-        <v>317</v>
+        <v>9553</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="n">
-        <v>2008</v>
+        <v>2016</v>
       </c>
       <c r="B3" s="2" t="n">
-        <v>43646</v>
+        <v>67839</v>
       </c>
       <c r="C3" s="2" t="n">
-        <v>50412</v>
+        <v>67984</v>
       </c>
       <c r="D3" s="2" t="n">
-        <v>17549</v>
+        <v>29021</v>
       </c>
       <c r="E3" s="2" t="n">
-        <v>2460</v>
+        <v>29441</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="n">
-        <v>2009</v>
+        <v>2017</v>
       </c>
       <c r="B4" s="2" t="n">
-        <v>42492</v>
+        <v>69607</v>
       </c>
       <c r="C4" s="2" t="n">
-        <v>46699</v>
+        <v>69573</v>
       </c>
       <c r="D4" s="2" t="n">
-        <v>17709</v>
+        <v>38910</v>
       </c>
       <c r="E4" s="2" t="n">
-        <v>2066</v>
+        <v>39822</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="n">
-        <v>2010</v>
+        <v>2018</v>
       </c>
       <c r="B5" s="2" t="n">
-        <v>43846</v>
+        <v>91785</v>
       </c>
       <c r="C5" s="2" t="n">
-        <v>50570</v>
+        <v>91741</v>
       </c>
       <c r="D5" s="2" t="n">
-        <v>29093</v>
+        <v>58853</v>
       </c>
       <c r="E5" s="2" t="n">
-        <v>3614</v>
+        <v>60533</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="n">
-        <v>2011</v>
+        <v>2019</v>
       </c>
       <c r="B6" s="2" t="n">
-        <v>47451</v>
+        <v>79181</v>
       </c>
       <c r="C6" s="2" t="n">
-        <v>55770</v>
+        <v>79217</v>
       </c>
       <c r="D6" s="2" t="n">
-        <v>36700</v>
+        <v>70823</v>
       </c>
       <c r="E6" s="2" t="n">
-        <v>4422</v>
+        <v>71879</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="n">
-        <v>2012</v>
+        <v>2020</v>
       </c>
       <c r="B7" s="2" t="n">
-        <v>48243</v>
+        <v>75590</v>
       </c>
       <c r="C7" s="2" t="n">
-        <v>57960</v>
+        <v>75618</v>
       </c>
       <c r="D7" s="2" t="n">
-        <v>44153</v>
+        <v>87477</v>
       </c>
       <c r="E7" s="2" t="n">
-        <v>4966</v>
+        <v>88389</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="n">
-        <v>2013</v>
+        <v>2021</v>
       </c>
       <c r="B8" s="2" t="n">
-        <v>51510</v>
+        <v>86687</v>
       </c>
       <c r="C8" s="2" t="n">
-        <v>58804</v>
+        <v>86818</v>
       </c>
       <c r="D8" s="2" t="n">
-        <v>59954</v>
+        <v>54299</v>
       </c>
       <c r="E8" s="2" t="n">
-        <v>5990</v>
+        <v>56111</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="n">
-        <v>2014</v>
+        <v>2022</v>
       </c>
       <c r="B9" s="2" t="n">
-        <v>50658</v>
+        <v>102464</v>
       </c>
       <c r="C9" s="2" t="n">
-        <v>62384</v>
+        <v>102400</v>
       </c>
       <c r="D9" s="2" t="n">
-        <v>66837</v>
+        <v>17075</v>
       </c>
       <c r="E9" s="2" t="n">
-        <v>5492</v>
-      </c>
-    </row>
-    <row r="10">
-      <c r="A10" s="2" t="n">
-        <v>2015</v>
-      </c>
-      <c r="B10" s="2" t="n">
-        <v>52696</v>
-      </c>
-      <c r="C10" s="2" t="n">
-        <v>62322</v>
-      </c>
-      <c r="D10" s="2" t="n">
-        <v>70039</v>
-      </c>
-      <c r="E10" s="2" t="n">
-        <v>5375</v>
-      </c>
-    </row>
-    <row r="11">
-      <c r="A11" s="2" t="n">
-        <v>2016</v>
-      </c>
-      <c r="B11" s="2" t="n">
-        <v>62675</v>
-      </c>
-      <c r="C11" s="2" t="n">
-        <v>66817</v>
-      </c>
-      <c r="D11" s="2" t="n">
-        <v>75145</v>
-      </c>
-      <c r="E11" s="2" t="n">
-        <v>7219</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="2" t="n">
-        <v>2017</v>
-      </c>
-      <c r="B12" s="2" t="n">
-        <v>60935</v>
-      </c>
-      <c r="C12" s="2" t="n">
-        <v>72460</v>
-      </c>
-      <c r="D12" s="2" t="n">
-        <v>82823</v>
-      </c>
-      <c r="E12" s="2" t="n">
-        <v>8105</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="2" t="n">
-        <v>2018</v>
-      </c>
-      <c r="B13" s="2" t="n">
-        <v>58335</v>
-      </c>
-      <c r="C13" s="2" t="n">
-        <v>76879</v>
-      </c>
-      <c r="D13" s="2" t="n">
-        <v>131701</v>
-      </c>
-      <c r="E13" s="2" t="n">
-        <v>10062</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="2" t="n">
-        <v>2019</v>
-      </c>
-      <c r="B14" s="2" t="n">
-        <v>69467</v>
-      </c>
-      <c r="C14" s="2" t="n">
-        <v>85300</v>
-      </c>
-      <c r="D14" s="2" t="n">
-        <v>115086</v>
-      </c>
-      <c r="E14" s="2" t="n">
-        <v>9016</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="2" t="n">
-        <v>2020</v>
-      </c>
-      <c r="B15" s="2" t="n">
-        <v>73431</v>
-      </c>
-      <c r="C15" s="2" t="n">
-        <v>89791</v>
-      </c>
-      <c r="D15" s="2" t="n">
-        <v>102243</v>
-      </c>
-      <c r="E15" s="2" t="n">
-        <v>7113</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="2" t="n">
-        <v>2021</v>
-      </c>
-      <c r="B16" s="2" t="n">
-        <v>82690</v>
-      </c>
-      <c r="C16" s="2" t="n">
-        <v>100987</v>
-      </c>
-      <c r="D16" s="2" t="n">
-        <v>57623</v>
-      </c>
-      <c r="E16" s="2" t="n">
-        <v>3466</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="2" t="n">
-        <v>2022</v>
-      </c>
-      <c r="B17" s="2" t="n">
-        <v>91795</v>
-      </c>
-      <c r="C17" s="2" t="n">
-        <v>116651</v>
-      </c>
-      <c r="D17" s="2" t="n">
-        <v>18294</v>
-      </c>
-      <c r="E17" s="2" t="n">
-        <v>1115</v>
+        <v>17255</v>
       </c>
     </row>
   </sheetData>
@@ -751,7 +615,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:E24"/>
+  <dimension ref="A1:E11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -759,7 +623,7 @@
   </sheetViews>
   <sheetFormatPr baseColWidth="8" defaultRowHeight="15"/>
   <cols>
-    <col width="16.22" customWidth="1" min="1" max="1"/>
+    <col width="15.22" customWidth="1" min="1" max="1"/>
     <col width="16.22" customWidth="1" min="2" max="2"/>
     <col width="1.22" customWidth="1" min="3" max="3"/>
     <col width="16.22" customWidth="1" min="4" max="4"/>
@@ -792,11 +656,11 @@
     <row r="2">
       <c r="A2" s="2" t="inlineStr">
         <is>
-          <t>Воронеж</t>
+          <t>Алматы</t>
         </is>
       </c>
       <c r="B2" s="2" t="n">
-        <v>73587</v>
+        <v>38699</v>
       </c>
       <c r="D2" s="2" t="inlineStr">
         <is>
@@ -804,17 +668,17 @@
         </is>
       </c>
       <c r="E2" s="3" t="n">
-        <v>0.2461</v>
+        <v>0.2514</v>
       </c>
     </row>
     <row r="3">
       <c r="A3" s="2" t="inlineStr">
         <is>
-          <t>Ростов-на-Дону</t>
+          <t>Нур-Султан</t>
         </is>
       </c>
       <c r="B3" s="2" t="n">
-        <v>76579</v>
+        <v>48521</v>
       </c>
       <c r="D3" s="2" t="inlineStr">
         <is>
@@ -822,89 +686,89 @@
         </is>
       </c>
       <c r="E3" s="3" t="n">
-        <v>0.1086</v>
+        <v>0.1105</v>
       </c>
     </row>
     <row r="4">
       <c r="A4" s="2" t="inlineStr">
         <is>
-          <t>Казань</t>
+          <t>Воронеж</t>
         </is>
       </c>
       <c r="B4" s="2" t="n">
-        <v>59991</v>
+        <v>56993</v>
       </c>
       <c r="D4" s="2" t="inlineStr">
         <is>
-          <t>Нижний Новгород</t>
+          <t>Новосибирск</t>
         </is>
       </c>
       <c r="E4" s="3" t="n">
-        <v>0.022</v>
+        <v>0.0316</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" s="2" t="inlineStr">
         <is>
-          <t>Нижний Новгород</t>
+          <t>Уфа</t>
         </is>
       </c>
       <c r="B5" s="2" t="n">
-        <v>76491</v>
+        <v>57608</v>
       </c>
       <c r="D5" s="2" t="inlineStr">
         <is>
-          <t>Ростов-на-Дону</t>
+          <t>Минск</t>
         </is>
       </c>
       <c r="E5" s="3" t="n">
-        <v>0.02</v>
+        <v>0.0276</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" s="2" t="inlineStr">
         <is>
-          <t>Новосибирск</t>
+          <t>Красноярск</t>
         </is>
       </c>
       <c r="B6" s="2" t="n">
-        <v>46820</v>
+        <v>58111</v>
       </c>
       <c r="D6" s="2" t="inlineStr">
         <is>
-          <t>Воронеж</t>
+          <t>Екатеринбург</t>
         </is>
       </c>
       <c r="E6" s="3" t="n">
-        <v>0.0167</v>
+        <v>0.0234</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" s="2" t="inlineStr">
         <is>
-          <t>Екатеринбург</t>
+          <t>Пермь</t>
         </is>
       </c>
       <c r="B7" s="2" t="n">
-        <v>81550</v>
+        <v>59927</v>
       </c>
       <c r="D7" s="2" t="inlineStr">
         <is>
-          <t>Екатеринбург</t>
+          <t>Алматы</t>
         </is>
       </c>
       <c r="E7" s="3" t="n">
-        <v>0.0305</v>
+        <v>0.022</v>
       </c>
     </row>
     <row r="8">
       <c r="A8" s="2" t="inlineStr">
         <is>
-          <t>Санкт-Петербург</t>
+          <t>Ростов-на-Дону</t>
         </is>
       </c>
       <c r="B8" s="2" t="n">
-        <v>52774</v>
+        <v>61013</v>
       </c>
       <c r="D8" s="2" t="inlineStr">
         <is>
@@ -912,239 +776,61 @@
         </is>
       </c>
       <c r="E8" s="3" t="n">
-        <v>0.0269</v>
+        <v>0.0217</v>
       </c>
     </row>
     <row r="9">
       <c r="A9" s="2" t="inlineStr">
         <is>
-          <t>Москва</t>
+          <t>Челябинск</t>
         </is>
       </c>
       <c r="B9" s="2" t="n">
-        <v>51234</v>
+        <v>61145</v>
       </c>
       <c r="D9" s="2" t="inlineStr">
         <is>
-          <t>Новосибирск</t>
+          <t>Краснодар</t>
         </is>
       </c>
       <c r="E9" s="3" t="n">
-        <v>0.0308</v>
+        <v>0.0201</v>
       </c>
     </row>
     <row r="10">
       <c r="A10" s="2" t="inlineStr">
         <is>
-          <t>Россия</t>
+          <t>Краснодар</t>
         </is>
       </c>
       <c r="B10" s="2" t="n">
-        <v>48221</v>
+        <v>64400</v>
       </c>
       <c r="D10" s="2" t="inlineStr">
         <is>
-          <t>Россия</t>
+          <t>Нижний Новгород</t>
         </is>
       </c>
       <c r="E10" s="3" t="n">
-        <v>0.0224</v>
+        <v>0.0182</v>
       </c>
     </row>
     <row r="11">
       <c r="A11" s="2" t="inlineStr">
         <is>
-          <t>Самара</t>
+          <t>Томск</t>
         </is>
       </c>
       <c r="B11" s="2" t="n">
-        <v>78886</v>
+        <v>69552</v>
       </c>
       <c r="D11" s="2" t="inlineStr">
         <is>
-          <t>Самара</t>
+          <t>Ростов-на-Дону</t>
         </is>
       </c>
       <c r="E11" s="3" t="n">
-        <v>0.0162</v>
-      </c>
-    </row>
-    <row r="12">
-      <c r="A12" s="2" t="inlineStr">
-        <is>
-          <t>Ярославль</t>
-        </is>
-      </c>
-      <c r="B12" s="2" t="n">
-        <v>46273</v>
-      </c>
-      <c r="D12" s="2" t="inlineStr">
-        <is>
-          <t>Краснодар</t>
-        </is>
-      </c>
-      <c r="E12" s="2" t="n">
-        <v>0.0243</v>
-      </c>
-    </row>
-    <row r="13">
-      <c r="A13" s="2" t="inlineStr">
-        <is>
-          <t>Краснодар</t>
-        </is>
-      </c>
-      <c r="B13" s="2" t="n">
-        <v>82585</v>
-      </c>
-      <c r="D13" s="2" t="inlineStr">
-        <is>
-          <t>Ярославль</t>
-        </is>
-      </c>
-      <c r="E13" s="2" t="n">
-        <v>0.0127</v>
-      </c>
-    </row>
-    <row r="14">
-      <c r="A14" s="2" t="inlineStr">
-        <is>
-          <t>Пермь</t>
-        </is>
-      </c>
-      <c r="B14" s="2" t="n">
-        <v>81440</v>
-      </c>
-      <c r="D14" s="2" t="inlineStr">
-        <is>
-          <t>Красноярск</t>
-        </is>
-      </c>
-      <c r="E14" s="2" t="n">
-        <v>0.0145</v>
-      </c>
-    </row>
-    <row r="15">
-      <c r="A15" s="2" t="inlineStr">
-        <is>
-          <t>Красноярск</t>
-        </is>
-      </c>
-      <c r="B15" s="2" t="n">
-        <v>69883</v>
-      </c>
-      <c r="D15" s="2" t="inlineStr">
-        <is>
-          <t>Пермь</t>
-        </is>
-      </c>
-      <c r="E15" s="2" t="n">
-        <v>0.0165</v>
-      </c>
-    </row>
-    <row r="16">
-      <c r="A16" s="2" t="inlineStr">
-        <is>
-          <t>Волгоград</t>
-        </is>
-      </c>
-      <c r="B16" s="2" t="n">
-        <v>46518</v>
-      </c>
-      <c r="D16" s="2" t="inlineStr">
-        <is>
-          <t>Уфа</t>
-        </is>
-      </c>
-      <c r="E16" s="2" t="n">
-        <v>0.0152</v>
-      </c>
-    </row>
-    <row r="17">
-      <c r="A17" s="2" t="inlineStr">
-        <is>
-          <t>Уфа</t>
-        </is>
-      </c>
-      <c r="B17" s="2" t="n">
-        <v>79632</v>
-      </c>
-      <c r="D17" s="2" t="inlineStr">
-        <is>
-          <t>Челябинск</t>
-        </is>
-      </c>
-      <c r="E17" s="2" t="n">
-        <v>0.0167</v>
-      </c>
-    </row>
-    <row r="18">
-      <c r="A18" s="2" t="inlineStr">
-        <is>
-          <t>Саратов</t>
-        </is>
-      </c>
-      <c r="B18" s="2" t="n">
-        <v>50935</v>
-      </c>
-    </row>
-    <row r="19">
-      <c r="A19" s="2" t="inlineStr">
-        <is>
-          <t>Тула</t>
-        </is>
-      </c>
-      <c r="B19" s="2" t="n">
-        <v>44614</v>
-      </c>
-    </row>
-    <row r="20">
-      <c r="A20" s="2" t="inlineStr">
-        <is>
-          <t>Ижевск</t>
-        </is>
-      </c>
-      <c r="B20" s="2" t="n">
-        <v>44443</v>
-      </c>
-    </row>
-    <row r="21">
-      <c r="A21" s="2" t="inlineStr">
-        <is>
-          <t>Челябинск</t>
-        </is>
-      </c>
-      <c r="B21" s="2" t="n">
-        <v>70440</v>
-      </c>
-    </row>
-    <row r="22">
-      <c r="A22" s="2" t="inlineStr">
-        <is>
-          <t>Омск</t>
-        </is>
-      </c>
-      <c r="B22" s="2" t="n">
-        <v>49788</v>
-      </c>
-    </row>
-    <row r="23">
-      <c r="A23" s="2" t="inlineStr">
-        <is>
-          <t>Рязань</t>
-        </is>
-      </c>
-      <c r="B23" s="2" t="n">
-        <v>37293</v>
-      </c>
-    </row>
-    <row r="24">
-      <c r="A24" s="2" t="inlineStr">
-        <is>
-          <t>Тюмень</t>
-        </is>
-      </c>
-      <c r="B24" s="2" t="n">
-        <v>78655</v>
+        <v>0.0181</v>
       </c>
     </row>
   </sheetData>

</xml_diff>